<commit_message>
Agenda week 1 "Toegevoegd" + Sjablonen agenda + notulen
</commit_message>
<xml_diff>
--- a/Opdrachten/sjabloon agenda.xlsx
+++ b/Opdrachten/sjabloon agenda.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26101"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2015-2016\Excel\Klas 2\Barroc-IT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/BarrocIT/Opdrachten/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="19440" windowHeight="11760"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="33740" windowHeight="19680"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -26,7 +31,7 @@
     <author>Fer</author>
   </authors>
   <commentList>
-    <comment ref="E3" authorId="0" shapeId="0">
+    <comment ref="E3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0">
+    <comment ref="B4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -74,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H19" authorId="0" shapeId="0">
+    <comment ref="H19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -103,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>wie</t>
   </si>
@@ -171,13 +176,16 @@
     <t>Welkom, vaststellen voorzitter + notulist , vaststellen definitieve agenda</t>
   </si>
   <si>
-    <t>Datum:25 aug.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Notulen aan :Fer, Sietse, Piet  </t>
   </si>
   <si>
-    <t xml:space="preserve"> AGENDA Barroc-IT Groep</t>
+    <t xml:space="preserve"> AGENDA Barroc-IT Groep 5</t>
+  </si>
+  <si>
+    <t>Datum: 8 sep.</t>
+  </si>
+  <si>
+    <t>Planning (vooruitzicht)</t>
   </si>
 </sst>
 </file>
@@ -295,14 +303,14 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -310,33 +318,33 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -345,7 +353,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -353,17 +361,17 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -373,7 +381,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -381,12 +389,12 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -395,55 +403,55 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -578,7 +586,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -594,9 +602,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -634,7 +642,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -706,7 +714,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -880,32 +888,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="168" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.86328125" customWidth="1"/>
-    <col min="2" max="2" width="9.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.86328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.86328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="77" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.265625" customWidth="1"/>
-    <col min="8" max="8" width="34.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.73046875" customWidth="1"/>
-    <col min="10" max="10" width="5.59765625" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" customWidth="1"/>
+    <col min="8" max="8" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.6640625" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" customWidth="1"/>
     <col min="16" max="16" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="52"/>
       <c r="C2" s="53"/>
       <c r="D2" s="53"/>
@@ -915,21 +923,21 @@
       <c r="H2" s="54"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="55" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="56"/>
       <c r="D3" s="57"/>
       <c r="E3" s="58" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" s="59"/>
       <c r="G3" s="59"/>
       <c r="H3" s="60"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="67" t="s">
         <v>19</v>
       </c>
@@ -941,9 +949,9 @@
       <c r="H4" s="63"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="70" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C5" s="71"/>
       <c r="D5" s="72"/>
@@ -953,7 +961,7 @@
       <c r="H5" s="66"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
@@ -971,7 +979,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="2:10" ht="17.649999999999999" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:10" ht="18" x14ac:dyDescent="0.2">
       <c r="B7" s="12"/>
       <c r="C7" s="13"/>
       <c r="D7" s="14"/>
@@ -981,9 +989,11 @@
       <c r="H7" s="18"/>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="C8" s="13">
+        <v>5</v>
+      </c>
       <c r="D8" s="13" t="s">
         <v>13</v>
       </c>
@@ -998,9 +1008,11 @@
       <c r="I8" s="19"/>
       <c r="J8" s="20"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+      <c r="C9" s="13">
+        <v>10</v>
+      </c>
       <c r="D9" s="13" t="s">
         <v>13</v>
       </c>
@@ -1013,21 +1025,25 @@
       <c r="H9" s="18"/>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
+      <c r="C10" s="13">
+        <v>10</v>
+      </c>
       <c r="D10" s="22" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E10" s="15">
         <v>3</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="21" t="s">
+        <v>25</v>
+      </c>
       <c r="G10" s="17"/>
       <c r="H10" s="18"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="22"/>
@@ -1038,7 +1054,7 @@
       <c r="H11" s="25"/>
       <c r="I11" s="19"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="22"/>
@@ -1050,7 +1066,7 @@
       <c r="H12" s="25"/>
       <c r="I12" s="19"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
       <c r="D13" s="22"/>
@@ -1062,7 +1078,7 @@
       <c r="H13" s="25"/>
       <c r="I13" s="19"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
       <c r="D14" s="22"/>
@@ -1074,7 +1090,7 @@
       <c r="H14" s="25"/>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
       <c r="D15" s="22" t="s">
@@ -1088,9 +1104,11 @@
       <c r="H15" s="18"/>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="22"/>
-      <c r="C16" s="13"/>
+      <c r="C16" s="13">
+        <v>5</v>
+      </c>
       <c r="D16" s="22" t="s">
         <v>5</v>
       </c>
@@ -1104,7 +1122,7 @@
       <c r="H16" s="18"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
       <c r="D17" s="27"/>
@@ -1113,11 +1131,11 @@
       <c r="G17" s="30"/>
       <c r="H17" s="31"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B18" s="32"/>
       <c r="C18" s="33">
         <f>SUM(C8:C17)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D18" s="33" t="s">
         <v>7</v>
@@ -1131,7 +1149,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B19" s="37"/>
       <c r="C19" s="33"/>
       <c r="D19" s="38" t="s">
@@ -1143,10 +1161,10 @@
       <c r="F19" s="39"/>
       <c r="G19" s="39"/>
       <c r="H19" s="36" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B20" s="37"/>
       <c r="C20" s="33"/>
       <c r="D20" s="38" t="s">
@@ -1159,7 +1177,7 @@
       <c r="G20" s="39"/>
       <c r="H20" s="40"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B21" s="37"/>
       <c r="C21" s="33"/>
       <c r="D21" s="38" t="s">
@@ -1172,7 +1190,7 @@
       <c r="G21" s="39"/>
       <c r="H21" s="40"/>
     </row>
-    <row r="22" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="41"/>
       <c r="C22" s="42"/>
       <c r="D22" s="43" t="s">
@@ -1185,12 +1203,12 @@
       <c r="G22" s="45"/>
       <c r="H22" s="46"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E24" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B25" s="47"/>
       <c r="E25" s="4">
         <v>1</v>
@@ -1198,7 +1216,7 @@
       <c r="F25" s="48"/>
       <c r="I25" s="49"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C26" s="1"/>
       <c r="E26" s="4">
         <v>2</v>
@@ -1206,7 +1224,7 @@
       <c r="F26" s="21"/>
       <c r="I26" s="49"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C27" s="1"/>
       <c r="E27" s="4">
         <v>3</v>
@@ -1214,7 +1232,7 @@
       <c r="F27" s="23"/>
       <c r="I27" s="49"/>
     </row>
-    <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28"/>
       <c r="D28" s="3"/>
       <c r="E28" s="4">
@@ -1225,14 +1243,14 @@
       <c r="H28" s="50"/>
       <c r="I28" s="51"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="E29" s="4">
         <v>5</v>
       </c>
       <c r="I29" s="49"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="E30" s="4">
         <v>6</v>
@@ -1240,7 +1258,7 @@
       <c r="F30" s="48"/>
       <c r="I30" s="49"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="E31" s="4">
         <v>7</v>
@@ -1248,18 +1266,18 @@
       <c r="F31" s="48"/>
       <c r="I31" s="49"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="F32" s="48"/>
       <c r="I32" s="49"/>
     </row>
-    <row r="33" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E33" s="4" t="s">
         <v>17</v>
       </c>
       <c r="I33" s="49"/>
     </row>
-    <row r="34" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E34" s="4">
         <v>1</v>
       </c>
@@ -1269,7 +1287,7 @@
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
     </row>
-    <row r="35" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E35" s="4">
         <v>2</v>
       </c>
@@ -1279,7 +1297,7 @@
       <c r="K35" s="21"/>
       <c r="L35" s="21"/>
     </row>
-    <row r="36" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E36" s="4">
         <v>3</v>
       </c>
@@ -1288,76 +1306,76 @@
       <c r="K36" s="21"/>
       <c r="L36" s="21"/>
     </row>
-    <row r="37" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I37" s="5"/>
     </row>
-    <row r="38" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I38" s="5"/>
     </row>
-    <row r="39" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I39" s="5"/>
     </row>
-    <row r="40" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I40" s="5"/>
     </row>
-    <row r="41" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I41" s="5"/>
     </row>
-    <row r="42" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I42" s="5"/>
     </row>
-    <row r="43" spans="5:12" x14ac:dyDescent="0.45">
+    <row r="43" spans="5:12" x14ac:dyDescent="0.2">
       <c r="I43" s="5"/>
     </row>
-    <row r="44" spans="5:12" x14ac:dyDescent="0.45">
+    <row r="44" spans="5:12" x14ac:dyDescent="0.2">
       <c r="I44" s="5"/>
     </row>
-    <row r="45" spans="5:12" x14ac:dyDescent="0.45">
+    <row r="45" spans="5:12" x14ac:dyDescent="0.2">
       <c r="I45" s="5"/>
     </row>
-    <row r="46" spans="5:12" x14ac:dyDescent="0.45">
+    <row r="46" spans="5:12" x14ac:dyDescent="0.2">
       <c r="I46" s="5"/>
     </row>
-    <row r="47" spans="5:12" x14ac:dyDescent="0.45">
+    <row r="47" spans="5:12" x14ac:dyDescent="0.2">
       <c r="I47" s="5"/>
     </row>
-    <row r="48" spans="5:12" x14ac:dyDescent="0.45">
+    <row r="48" spans="5:12" x14ac:dyDescent="0.2">
       <c r="I48" s="5"/>
     </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I49" s="5"/>
     </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I50" s="5"/>
     </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I51" s="5"/>
     </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I52" s="5"/>
     </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I53" s="5"/>
     </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I54" s="5"/>
     </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I55" s="5"/>
     </row>
-    <row r="56" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I56" s="5"/>
     </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I57" s="5"/>
     </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I58" s="5"/>
     </row>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I59" s="5"/>
     </row>
-    <row r="60" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I60" s="5"/>
     </row>
   </sheetData>
@@ -1380,7 +1398,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1392,7 +1410,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1448,18 +1466,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1478,17 +1496,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D4A539-5E71-46A4-A076-A8448D6640BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EC78C7E-41AD-4518-BFAA-0ABA4B09AB48}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D4A539-5E71-46A4-A076-A8448D6640BC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>